<commit_message>
add order metadata to add metadata pipeline
</commit_message>
<xml_diff>
--- a/src/test/resources/net/pageseeder/ox/web/mps4/addmetadata/basic/embargo-add-metadata-test.xlsx
+++ b/src/test/resources/net/pageseeder/ox/web/mps4/addmetadata/basic/embargo-add-metadata-test.xlsx
@@ -1,37 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\pbs\berliozweb-mps4-ox-models\src\test\resources\net\pageseeder\ox\web\mps4\addmetadata\basic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892C9826-3839-4D5E-810D-5D9B7FF4AE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978AFFA7-B2C0-4EB7-AB08-33E1B77F4062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="28800" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="files" sheetId="1" r:id="rId1"/>
     <sheet name="metadata" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>Last modified</t>
   </si>
@@ -124,6 +114,12 @@
   </si>
   <si>
     <t>_chemoc</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>_embargo</t>
   </si>
 </sst>
 </file>
@@ -623,7 +619,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -638,6 +634,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -684,7 +683,11 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-C09]dd/mmm/yy;@"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -737,37 +740,38 @@
     <sortCondition ref="C1:C4"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Last modified" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Year metadata" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Last modified" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Year metadata" dataDxfId="8"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Folder"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="File name"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column2" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column2" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="A1:K4" totalsRowShown="0">
-  <autoFilter ref="A1:K4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="A1:L4" totalsRowShown="0">
+  <autoFilter ref="A1:L4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J4">
     <sortCondition ref="G1:G4"/>
   </sortState>
-  <tableColumns count="11">
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="URIID" dataDxfId="5"/>
+  <tableColumns count="12">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="URIID" dataDxfId="6"/>
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="year"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="month" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="value" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="month" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="value" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="title"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Publication"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="path"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="filename"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="media" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="pub-date" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Description" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="media" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="pub-date" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Description" dataDxfId="1">
       <calculatedColumnFormula>_xlfn.CONCAT(Table3[[#This Row],[Publication]],"    ",Table3[[#This Row],[media]])</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="12" xr3:uid="{0D455CA7-4EE5-4D0A-97E2-4AC0F4CAFA3D}" name="order" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1062,7 +1066,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1179,10 +1183,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1197,9 +1201,10 @@
     <col min="9" max="9" width="11.28515625" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
     <col min="11" max="11" width="84" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.25" customHeight="1">
+    <row r="1" spans="1:12" ht="14.25" customHeight="1">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -1233,8 +1238,11 @@
       <c r="K1" t="s">
         <v>20</v>
       </c>
+      <c r="L1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="14.25" customHeight="1">
+    <row r="2" spans="1:12" ht="14.25" customHeight="1">
       <c r="A2" t="e">
         <f>INDEX(Table1[ID],MATCH(Table1[Year metadata],Table3[value],0))</f>
         <v>#N/A</v>
@@ -1270,8 +1278,11 @@
         <f>_xlfn.CONCAT(Table3[[#This Row],[Publication]],"    ",Table3[[#This Row],[media]])</f>
         <v>- published 6 December 2019    pdf</v>
       </c>
+      <c r="L2" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" ht="14.25" customHeight="1">
+    <row r="3" spans="1:12" ht="14.25" customHeight="1">
       <c r="A3">
         <f>INDEX(Table1[ID],MATCH(Table1[Year metadata],Table3[value],0))</f>
         <v>110605</v>
@@ -1307,8 +1318,11 @@
         <f>_xlfn.CONCAT(Table3[[#This Row],[Publication]],"    ",Table3[[#This Row],[media]])</f>
         <v>- published 6 December 2019    pdf</v>
       </c>
+      <c r="L3" s="9">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12">
       <c r="A4">
         <f>INDEX(Table1[ID],MATCH(Table1[Year metadata],Table3[value],0))</f>
         <v>110603</v>
@@ -1329,7 +1343,7 @@
         <v>7</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="H4" t="s">
         <v>23</v>
@@ -1343,6 +1357,9 @@
       <c r="K4" s="6" t="str">
         <f>_xlfn.CONCAT(Table3[[#This Row],[Publication]],"    ",Table3[[#This Row],[media]])</f>
         <v>- published 6 December 2019    pdf</v>
+      </c>
+      <c r="L4" s="9">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the description logic for add metadata pipeline
</commit_message>
<xml_diff>
--- a/src/test/resources/net/pageseeder/ox/web/mps4/addmetadata/basic/embargo-add-metadata-test.xlsx
+++ b/src/test/resources/net/pageseeder/ox/web/mps4/addmetadata/basic/embargo-add-metadata-test.xlsx
@@ -8,45 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\pbs\berliozweb-mps4-ox-models\src\test\resources\net\pageseeder\ox\web\mps4\addmetadata\basic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978AFFA7-B2C0-4EB7-AB08-33E1B77F4062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C24500-219D-4DF8-948F-90F6FCDAD902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="28800" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="files" sheetId="1" r:id="rId1"/>
-    <sheet name="metadata" sheetId="2" r:id="rId2"/>
+    <sheet name="metadata" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
-  <si>
-    <t>Last modified</t>
-  </si>
-  <si>
-    <t>Year metadata</t>
-  </si>
-  <si>
-    <t>Folder</t>
-  </si>
-  <si>
-    <t>File name</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
-    <t>2020-01</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Efficient Funding of Chemotherapy Supplement Summary of Changes</t>
   </si>
   <si>
-    <t>- published 6 December 2019</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -56,63 +34,30 @@
     <t>month</t>
   </si>
   <si>
-    <t>value</t>
-  </si>
-  <si>
     <t>path</t>
   </si>
   <si>
     <t>filename</t>
   </si>
   <si>
-    <t>media</t>
-  </si>
-  <si>
     <t>pub-date</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>pdf</t>
-  </si>
-  <si>
     <t>URIID</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Publication</t>
-  </si>
-  <si>
-    <t>2020-01  /  2020-01-01-efc-soc-r2-b3-test-01.pdf</t>
-  </si>
-  <si>
-    <t>2020-01-01-efc-soc-r2-b3-test-01.pdf</t>
-  </si>
-  <si>
-    <t>/ps/data_source/files/documents/embargo/test/01</t>
-  </si>
-  <si>
-    <t>2020-01  /  invalid-file.pdf</t>
-  </si>
-  <si>
     <t>invalid-file.pdf</t>
   </si>
   <si>
-    <t>2020-01  / invalid-file.pdf</t>
-  </si>
-  <si>
     <t>2020-01-01-efc-soc-r2-b3-test_chemoc.pdf</t>
   </si>
   <si>
-    <t>2020-01  /  2020-01-01-efc-soc-r2-b3-test_chemoc.pdf</t>
-  </si>
-  <si>
     <t>_chemoc</t>
   </si>
   <si>
@@ -120,6 +65,48 @@
   </si>
   <si>
     <t>_embargo</t>
+  </si>
+  <si>
+    <t>Chemo example</t>
+  </si>
+  <si>
+    <t>Embargo without description</t>
+  </si>
+  <si>
+    <t>Will be ignored</t>
+  </si>
+  <si>
+    <t>invalid uriid</t>
+  </si>
+  <si>
+    <t>Embargo with description</t>
+  </si>
+  <si>
+    <t>Description example</t>
+  </si>
+  <si>
+    <t>2020-01-01-efc-soc-r2-b3-test_embargo-no-description.pdf</t>
+  </si>
+  <si>
+    <t>2020-01-01-efc-soc-r2-b3-test_embargo-with-description.pdf</t>
+  </si>
+  <si>
+    <t>2020-01-01-efc-soc-r2-b3-test_offline.pdf</t>
+  </si>
+  <si>
+    <t>_offline</t>
+  </si>
+  <si>
+    <t>Offline Example</t>
+  </si>
+  <si>
+    <t>2020-01-01-efc-soc-r2-b3-test_sqlite.pdf</t>
+  </si>
+  <si>
+    <t>_sqlite</t>
+  </si>
+  <si>
+    <t>Sqlite example</t>
   </si>
 </sst>
 </file>
@@ -130,7 +117,7 @@
     <numFmt numFmtId="164" formatCode="00"/>
     <numFmt numFmtId="165" formatCode="[$-C09]dd/mmm/yy;@"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,12 +248,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -459,7 +440,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -574,6 +555,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -619,23 +609,30 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
@@ -683,42 +680,278 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="10">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="165" formatCode="[$-C09]dd/mmm/yy;@"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="165" formatCode="[$-C09]dd/mmm/yy;@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="00"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="dd/mm/yy\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -734,46 +967,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F4" totalsRowShown="0">
-  <autoFilter ref="A1:F4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F4">
-    <sortCondition ref="C1:C4"/>
-  </sortState>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Last modified" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Year metadata" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Folder"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="File name"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column2" dataDxfId="7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00FFD996-A730-4A74-8CAC-366A55B3390E}" name="Table1" displayName="Table1" ref="A1:I7" totalsRowShown="0" tableBorderDxfId="9">
+  <autoFilter ref="A1:I7" xr:uid="{00FFD996-A730-4A74-8CAC-366A55B3390E}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{25DE500C-0003-4E71-A1D3-F548F734E77E}" name="URIID" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{0B4CB7A8-D78E-4C86-AA0D-2BCBDAC44D79}" name="year" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{E09AEA31-46F3-464A-AD59-024E4FCB3916}" name="month" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{2B0C7405-BD00-4C32-9DFB-AB97AF136BE6}" name="title" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{798C5FF9-5A02-4F92-99C0-D06B98182FB9}" name="path" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{E3DBFF8F-F6A2-462E-A973-1A0EA2A4FF6E}" name="filename" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{774DDC8F-58D9-4C6C-92C2-2873B444261A}" name="pub-date" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{9CD9AD11-97E7-4752-9E64-504666B8A56A}" name="Description" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{112F464D-BCCD-4680-93C1-2D65B97508B0}" name="order" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="A1:L4" totalsRowShown="0">
-  <autoFilter ref="A1:L4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J4">
-    <sortCondition ref="G1:G4"/>
-  </sortState>
-  <tableColumns count="12">
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="URIID" dataDxfId="6"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="year"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="month" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="value" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="title"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Publication"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="path"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="filename"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="media" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="pub-date" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Description" dataDxfId="1">
-      <calculatedColumnFormula>_xlfn.CONCAT(Table3[[#This Row],[Publication]],"    ",Table3[[#This Row],[media]])</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="12" xr3:uid="{0D455CA7-4EE5-4D0A-97E2-4AC0F4CAFA3D}" name="order" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1073,300 +1280,227 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{368B7088-C282-4EFC-9180-5F01094FCE9E}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="80.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="8" width="70.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C2" s="2">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3">
+        <v>43257</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1">
+        <v>110902</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C3" s="2">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="3">
+        <v>43592</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1">
+        <v>110899</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2020</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="3">
+        <v>43929</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1">
+        <v>110903</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2021</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="3">
+        <v>44264</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1">
+        <v>110900</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2022</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="3">
+        <v>44602</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1">
+        <v>110901</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2023</v>
+      </c>
+      <c r="C7" s="2">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B2" s="1">
-        <v>44896.685208333336</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="5">
-        <v>110605</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44896.685208333336</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="5">
-        <v>110603</v>
-      </c>
-      <c r="B4" s="1">
-        <v>44896.685208333336</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="95" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="83.7109375" customWidth="1"/>
-    <col min="6" max="6" width="46.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="84" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A2" t="e">
-        <f>INDEX(Table1[ID],MATCH(Table1[Year metadata],Table3[value],0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="B2">
-        <v>2020</v>
-      </c>
-      <c r="C2" s="7">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G7" s="3">
+        <v>44937</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="6">
         <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="4">
-        <v>43805</v>
-      </c>
-      <c r="K2" s="6" t="str">
-        <f>_xlfn.CONCAT(Table3[[#This Row],[Publication]],"    ",Table3[[#This Row],[media]])</f>
-        <v>- published 6 December 2019    pdf</v>
-      </c>
-      <c r="L2" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A3">
-        <f>INDEX(Table1[ID],MATCH(Table1[Year metadata],Table3[value],0))</f>
-        <v>110605</v>
-      </c>
-      <c r="B3">
-        <v>2020</v>
-      </c>
-      <c r="C3" s="7">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="4">
-        <v>43805</v>
-      </c>
-      <c r="K3" s="6" t="str">
-        <f>_xlfn.CONCAT(Table3[[#This Row],[Publication]],"    ",Table3[[#This Row],[media]])</f>
-        <v>- published 6 December 2019    pdf</v>
-      </c>
-      <c r="L3" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4">
-        <f>INDEX(Table1[ID],MATCH(Table1[Year metadata],Table3[value],0))</f>
-        <v>110603</v>
-      </c>
-      <c r="B4">
-        <v>2020</v>
-      </c>
-      <c r="C4" s="7">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="4">
-        <v>43805</v>
-      </c>
-      <c r="K4" s="6" t="str">
-        <f>_xlfn.CONCAT(Table3[[#This Row],[Publication]],"    ",Table3[[#This Row],[media]])</f>
-        <v>- published 6 December 2019    pdf</v>
-      </c>
-      <c r="L4" s="9">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change the description logiv and removed the metadata pub-date
</commit_message>
<xml_diff>
--- a/src/test/resources/net/pageseeder/ox/web/mps4/addmetadata/basic/embargo-add-metadata-test.xlsx
+++ b/src/test/resources/net/pageseeder/ox/web/mps4/addmetadata/basic/embargo-add-metadata-test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\pbs\berliozweb-mps4-ox-models\src\test\resources\net\pageseeder\ox\web\mps4\addmetadata\basic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C24500-219D-4DF8-948F-90F6FCDAD902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B91379-F857-4640-8A6A-3ADF00D9D0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,30 +609,29 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
@@ -1284,7 +1283,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1297,31 +1296,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="7" t="s">
+      <c r="A1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>